<commit_message>
Auto update 2025-11-26 18:37:25
</commit_message>
<xml_diff>
--- a/bad_quality_photos.xlsx
+++ b/bad_quality_photos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,6 +448,1133 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0026-6</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\0026-6\1_image_0026-6.jpg</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1431</v>
+      </c>
+      <c r="D2" t="n">
+        <v>500</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0039-3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\0039-3\2_image_0039-3.jpg</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1211</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>005</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\005\5_image_005.jpg</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>884</v>
+      </c>
+      <c r="D4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>009-4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\009-4\7_image_009-4.jpg</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>873</v>
+      </c>
+      <c r="D5" t="n">
+        <v>500</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>3114</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\3114\6_image_3114.jpg</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1638</v>
+      </c>
+      <c r="D6" t="n">
+        <v>500</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>3131</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\3131\8_image_3131.jpg</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>997</v>
+      </c>
+      <c r="D7" t="n">
+        <v>500</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>3221 Місто</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\3221 Місто\8_image_3221 Місто.jpg</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1227</v>
+      </c>
+      <c r="D8" t="n">
+        <v>500</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>5302 Бордова</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\5302 Бордова\2_image_5302 Бордова.jpg</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1004</v>
+      </c>
+      <c r="D9" t="n">
+        <v>500</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>5302 Чорна</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\5302 Чорна\2_image_5302 Чорна.jpg</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1111</v>
+      </c>
+      <c r="D10" t="n">
+        <v>500</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BV12138-19-104</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\BV12138-19-104\2_image_BV12138-19-104.jpg</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>500</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1969</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>BV12374-011-24</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\BV12374-011-24\5_image_BV12374-011-24.jpg</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>500</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1018</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BV12374-011-28</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\BV12374-011-28\5_image_BV12374-011-28.jpg</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>500</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1018</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BV38363-100</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\BV38363-100\1_image_BV38363-100.jpg</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>829</v>
+      </c>
+      <c r="D14" t="n">
+        <v>500</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>C-3079A-pink</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C-3079A-pink\1_image_C-3079A-pink.jpg</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>968</v>
+      </c>
+      <c r="D15" t="n">
+        <v>500</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>C-3079A-pink</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C-3079A-pink\3_image_C-3079A-pink.jpg</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1010</v>
+      </c>
+      <c r="D16" t="n">
+        <v>500</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>C-3820A-red</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C-3820A-red\1_image_C-3820A-red.jpg</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1044</v>
+      </c>
+      <c r="D17" t="n">
+        <v>500</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>C-3820A-red</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C-3820A-red\6_image_C-3820A-red.jpg</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>821</v>
+      </c>
+      <c r="D18" t="n">
+        <v>500</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>C-6200A-black</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C-6200A-black\7_image_C-6200A-black.jpg</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>829</v>
+      </c>
+      <c r="D19" t="n">
+        <v>500</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>C-8460A-black</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C-8460A-black\1_image_C-8460A-black.jpg</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>978</v>
+      </c>
+      <c r="D20" t="n">
+        <v>500</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>C-8460A-silvery-grey</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C-8460A-silvery-grey\5_image_C-8460A-silvery-grey.jpg</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>884</v>
+      </c>
+      <c r="D21" t="n">
+        <v>500</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>C-8998-lime green</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C-8998-lime green\1_image_C-8998-lime green.jpg</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>953</v>
+      </c>
+      <c r="D22" t="n">
+        <v>500</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>C2-936-black</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C2-936-black\7_image_C2-936-black.jpg</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>841</v>
+      </c>
+      <c r="D23" t="n">
+        <v>500</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>C2-936-dark purple</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C2-936-dark purple\3_image_C2-936-dark purple.jpg</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1006</v>
+      </c>
+      <c r="D24" t="n">
+        <v>500</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>C2-936-red</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C2-936-red\3_image_C2-936-red.jpg</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D25" t="n">
+        <v>500</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>C34815-1</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C34815-1\1_image_C34815-1.jpg</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1055</v>
+      </c>
+      <c r="D26" t="n">
+        <v>500</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>C34815-1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C34815-1\8_image_C34815-1.jpg</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>911</v>
+      </c>
+      <c r="D27" t="n">
+        <v>500</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>C34815-4</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\C34815-4\1_image_C34815-4.jpg</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>933</v>
+      </c>
+      <c r="D28" t="n">
+        <v>500</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>DRS17116-3</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\DRS17116-3\4_image_DRS17116-3.jpg</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>1028</v>
+      </c>
+      <c r="D29" t="n">
+        <v>500</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>DRS19353-1</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\DRS19353-1\9_image_DRS19353-1.jpg</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>500</v>
+      </c>
+      <c r="D30" t="n">
+        <v>843</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>L20011-1</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L20011-1\5_image_L20011-1.jpg</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1057</v>
+      </c>
+      <c r="D31" t="n">
+        <v>500</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>L20030-1</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L20030-1\6_image_L20030-1.jpg</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>919</v>
+      </c>
+      <c r="D32" t="n">
+        <v>500</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>L20812-1</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L20812-1\5_image_L20812-1.jpg</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>944</v>
+      </c>
+      <c r="D33" t="n">
+        <v>500</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>L20812-10</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L20812-10\5_image_L20812-10.jpg</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D34" t="n">
+        <v>500</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>L21075-1</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L21075-1\1_image_L21075-1.jpg</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>1032</v>
+      </c>
+      <c r="D35" t="n">
+        <v>500</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>L22537-179</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L22537-179\3_image_L22537-179.jpg</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>937</v>
+      </c>
+      <c r="D36" t="n">
+        <v>500</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>L86913-1</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L86913-1\2_image_L86913-1.jpg</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>500</v>
+      </c>
+      <c r="D37" t="n">
+        <v>948</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>L86913-1</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L86913-1\4_image_L86913-1.jpg</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>947</v>
+      </c>
+      <c r="D38" t="n">
+        <v>500</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>L86913-1</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L86913-1\7_image_L86913-1.jpg</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>500</v>
+      </c>
+      <c r="D39" t="n">
+        <v>948</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>L86913-15</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L86913-15\4_image_L86913-15.jpg</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>841</v>
+      </c>
+      <c r="D40" t="n">
+        <v>500</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>L86913-15</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L86913-15\8_image_L86913-15.jpg</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>500</v>
+      </c>
+      <c r="D41" t="n">
+        <v>948</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>L86913-3</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L86913-3\7_image_L86913-3.jpg</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>500</v>
+      </c>
+      <c r="D42" t="n">
+        <v>948</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>L86963-10</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L86963-10\7_image_L86963-10.jpg</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>500</v>
+      </c>
+      <c r="D43" t="n">
+        <v>948</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>L86963-10</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L86963-10\8_image_L86963-10.jpg</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>873</v>
+      </c>
+      <c r="D44" t="n">
+        <v>500</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>L86963-14</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\L86963-14\7_image_L86963-14.jpg</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>500</v>
+      </c>
+      <c r="D45" t="n">
+        <v>948</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>LC45851X-2</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\LC45851X-2\1_image_LC45851X-2.jpg</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>724</v>
+      </c>
+      <c r="D46" t="n">
+        <v>500</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>LC47323-1</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\LC47323-1\1_image_LC47323-1.jpg</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>500</v>
+      </c>
+      <c r="D47" t="n">
+        <v>842</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>LC89049-F9976</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\LC89049-F9976\6_image_LC89049-F9976.jpg</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>1162</v>
+      </c>
+      <c r="D48" t="n">
+        <v>500</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>T37193-5056</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\T37193-5056\2_image_T37193-5056.jpg</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>500</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1785</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>T37193-5056</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/21212\T37193-5056\4_image_T37193-5056.jpg</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>1169</v>
+      </c>
+      <c r="D50" t="n">
+        <v>500</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto update 2025-11-28 08:35:58
</commit_message>
<xml_diff>
--- a/bad_quality_photos.xlsx
+++ b/bad_quality_photos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,16 +451,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0026-6</t>
+          <t>L26835-51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\0026-6\001_image_0026-6.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\L26835-51\3_image_L26835-51.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1431</v>
+        <v>970</v>
       </c>
       <c r="D2" t="n">
         <v>500</v>
@@ -474,19 +474,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0039-3</t>
+          <t>L87530-4Y</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\0039-3\003_image_0039-3.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\L87530-4Y\007_image_L87530-4Y.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>500</v>
+        <v>872</v>
       </c>
       <c r="D3" t="n">
-        <v>1211</v>
+        <v>500</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -497,16 +497,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>005</t>
+          <t>L88005-215</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\005\5_image_005.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\L88005-215\3_image_L88005-215.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D4" t="n">
         <v>500</v>
@@ -520,16 +520,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>009-4</t>
+          <t>L88530-1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\009-4\7_image_009-4.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\L88530-1\4_image_L88530-1.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>873</v>
+        <v>879</v>
       </c>
       <c r="D5" t="n">
         <v>500</v>
@@ -543,16 +543,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3114</t>
+          <t>L88542-1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\3114\6_image_3114.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\L88542-1\4_image_L88542-1.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1638</v>
+        <v>985</v>
       </c>
       <c r="D6" t="n">
         <v>500</v>
@@ -566,16 +566,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3131</t>
+          <t>L88542-65</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\3131\8_image_3131.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\L88542-65\007_image_L88542-65.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>997</v>
+        <v>833</v>
       </c>
       <c r="D7" t="n">
         <v>500</v>
@@ -589,16 +589,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3221 Місто</t>
+          <t>LC14052-YP2020</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\3221 Місто\8_image_3221 Місто.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC14052-YP2020\5_image_LC14052-YP2020.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1227</v>
+        <v>909</v>
       </c>
       <c r="D8" t="n">
         <v>500</v>
@@ -612,19 +612,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5302 Бордова</t>
+          <t>LC14621-GD02</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\5302 Бордова\002_image_5302 Бордова.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC14621-GD02\009_image_LC14621-GD02.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1004</v>
+        <v>500</v>
       </c>
       <c r="D9" t="n">
-        <v>500</v>
+        <v>847</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -635,16 +635,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5302 Чорна</t>
+          <t>LC14621-GD02</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\5302 Чорна\2_image_5302 Чорна.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC14621-GD02\4_image_LC14621-GD02.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1111</v>
+        <v>1029</v>
       </c>
       <c r="D10" t="n">
         <v>500</v>
@@ -658,19 +658,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BV12138-19-104</t>
+          <t>LC14621-GD04</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\BV12138-19-104\2_image_BV12138-19-104.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC14621-GD04\7_image_LC14621-GD04.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>500</v>
       </c>
       <c r="D11" t="n">
-        <v>1969</v>
+        <v>1051</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -681,19 +681,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BV12374-011-24</t>
+          <t>LC14621-GD22</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\BV12374-011-24\5_image_BV12374-011-24.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC14621-GD22\4_image_LC14621-GD22.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>500</v>
+        <v>828</v>
       </c>
       <c r="D12" t="n">
-        <v>1018</v>
+        <v>500</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -704,19 +704,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BV12374-011-28</t>
+          <t>LC14621-GD25</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\BV12374-011-28\5_image_BV12374-011-28.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC14621-GD25\5_image_LC14621-GD25.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>500</v>
+        <v>1188</v>
       </c>
       <c r="D13" t="n">
-        <v>1018</v>
+        <v>500</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -727,19 +727,19 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BV38363-100</t>
+          <t>LC14621-GD25</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\BV38363-100\1_image_BV38363-100.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC14621-GD25\7_image_LC14621-GD25.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>829</v>
+        <v>500</v>
       </c>
       <c r="D14" t="n">
-        <v>500</v>
+        <v>911</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -750,16 +750,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C-3079A-pink</t>
+          <t>LC14805-GD01</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C-3079A-pink\1_image_C-3079A-pink.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC14805-GD01\4_image_LC14805-GD01.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>968</v>
+        <v>1062</v>
       </c>
       <c r="D15" t="n">
         <v>500</v>
@@ -773,16 +773,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C-3079A-pink</t>
+          <t>LC14825-GD01</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C-3079A-pink\3_image_C-3079A-pink.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC14825-GD01\4_image_LC14825-GD01.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1010</v>
+        <v>955</v>
       </c>
       <c r="D16" t="n">
         <v>500</v>
@@ -796,16 +796,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C-3820A-red</t>
+          <t>LC68308-01</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C-3820A-red\1_image_C-3820A-red.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC68308-01\4_image_LC68308-01.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1044</v>
+        <v>997</v>
       </c>
       <c r="D17" t="n">
         <v>500</v>
@@ -819,16 +819,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C-3820A-red</t>
+          <t>LC68808-04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C-3820A-red\6_image_C-3820A-red.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC68808-04\008_image_LC68808-04.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="D18" t="n">
         <v>500</v>
@@ -842,16 +842,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C-6200A-black</t>
+          <t>LC68900-05</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C-6200A-black\7_image_C-6200A-black.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC68900-05\001_image_LC68900-05.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>829</v>
+        <v>857</v>
       </c>
       <c r="D19" t="n">
         <v>500</v>
@@ -865,16 +865,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C-8460A-black</t>
+          <t>LC68900-98</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C-8460A-black\1_image_C-8460A-black.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC68900-98\4_image_LC68900-98.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>978</v>
+        <v>992</v>
       </c>
       <c r="D20" t="n">
         <v>500</v>
@@ -888,16 +888,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>C-8460A-silvery-grey</t>
+          <t>LC89049-F9976</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C-8460A-silvery-grey\5_image_C-8460A-silvery-grey.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\LC89049-F9976\6_image_LC89049-F9976.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>884</v>
+        <v>1162</v>
       </c>
       <c r="D21" t="n">
         <v>500</v>
@@ -911,16 +911,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>C-8998-lime green</t>
+          <t>S31011-1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C-8998-lime green\1_image_C-8998-lime green.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\S31011-1\001_image_S31011-1.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>953</v>
+        <v>719</v>
       </c>
       <c r="D22" t="n">
         <v>500</v>
@@ -934,16 +934,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>C2-936-black</t>
+          <t>S31578-2</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C2-936-black\7_image_C2-936-black.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\S31578-2\001_image_S31578-2.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>841</v>
+        <v>889</v>
       </c>
       <c r="D23" t="n">
         <v>500</v>
@@ -957,16 +957,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>C2-936-dark purple</t>
+          <t>S31585-7</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C2-936-dark purple\3_image_C2-936-dark purple.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\S31585-7\001_image_S31585-7.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1006</v>
+        <v>909</v>
       </c>
       <c r="D24" t="n">
         <v>500</v>
@@ -980,16 +980,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>C2-936-red</t>
+          <t>W15614-green</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C2-936-red\3_image_C2-936-red.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\W15614-green\001_image_W15614-green.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1007</v>
+        <v>858</v>
       </c>
       <c r="D25" t="n">
         <v>500</v>
@@ -1003,16 +1003,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>C34815-1</t>
+          <t>Y-1088B-green</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C34815-1\1_image_C34815-1.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\Y-1088B-green\4_image_Y-1088B-green.jpg</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1055</v>
+        <v>905</v>
       </c>
       <c r="D26" t="n">
         <v>500</v>
@@ -1026,16 +1026,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>C34815-1</t>
+          <t>Y-7001A-lime-green-lak</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C34815-1\8_image_C34815-1.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\Y-7001A-lime-green-lak\3_image_Y-7001A-lime-green-lak.jpg</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>911</v>
+        <v>924</v>
       </c>
       <c r="D27" t="n">
         <v>500</v>
@@ -1049,16 +1049,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>C34815-4</t>
+          <t>Y-7001A-pink-lak</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\C34815-4\1_image_C34815-4.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\Y-7001A-pink-lak\3_image_Y-7001A-pink-lak.jpg</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>933</v>
+        <v>803</v>
       </c>
       <c r="D28" t="n">
         <v>500</v>
@@ -1072,16 +1072,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>DRS17116-3</t>
+          <t>Y-7767A-deep-purple</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\DRS17116-3\4_image_DRS17116-3.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\Y-7767A-deep-purple\001_image_Y-7767A-deep-purple.jpg</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1028</v>
+        <v>940</v>
       </c>
       <c r="D29" t="n">
         <v>500</v>
@@ -1095,19 +1095,19 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>DRS19353-1</t>
+          <t>Y-7767A-green</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\DRS19353-1\9_image_DRS19353-1.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\Y-7767A-green\3_image_Y-7767A-green.jpg</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>500</v>
+        <v>1006</v>
       </c>
       <c r="D30" t="n">
-        <v>843</v>
+        <v>500</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1118,16 +1118,16 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>L20011-1</t>
+          <t>Y-7767A-khaki</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\L20011-1\5_image_L20011-1.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\Y-7767A-khaki\001_image_Y-7767A-khaki.jpg</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1057</v>
+        <v>923</v>
       </c>
       <c r="D31" t="n">
         <v>500</v>
@@ -1141,435 +1141,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>L20030-1</t>
+          <t>Y-7767A-red</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\L20030-1\6_image_L20030-1.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\Y-7767A-red\001_image_Y-7767A-red.jpg</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>919</v>
+        <v>938</v>
       </c>
       <c r="D32" t="n">
         <v>500</v>
       </c>
       <c r="E32" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>L20812-1</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L20812-1\5_image_L20812-1.jpg</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>944</v>
-      </c>
-      <c r="D33" t="n">
-        <v>500</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>L20812-10</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L20812-10\5_image_L20812-10.jpg</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>1014</v>
-      </c>
-      <c r="D34" t="n">
-        <v>500</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>L21075-1</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L21075-1\1_image_L21075-1.jpg</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>1032</v>
-      </c>
-      <c r="D35" t="n">
-        <v>500</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>L22537-179</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L22537-179\3_image_L22537-179.jpg</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>937</v>
-      </c>
-      <c r="D36" t="n">
-        <v>500</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>L86913-1</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L86913-1\2_image_L86913-1.jpg</t>
-        </is>
-      </c>
-      <c r="C37" t="n">
-        <v>500</v>
-      </c>
-      <c r="D37" t="n">
-        <v>948</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>L86913-1</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L86913-1\4_image_L86913-1.jpg</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
-        <v>947</v>
-      </c>
-      <c r="D38" t="n">
-        <v>500</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>L86913-1</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L86913-1\7_image_L86913-1.jpg</t>
-        </is>
-      </c>
-      <c r="C39" t="n">
-        <v>500</v>
-      </c>
-      <c r="D39" t="n">
-        <v>948</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>L86913-15</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L86913-15\4_image_L86913-15.jpg</t>
-        </is>
-      </c>
-      <c r="C40" t="n">
-        <v>841</v>
-      </c>
-      <c r="D40" t="n">
-        <v>500</v>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>L86913-15</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L86913-15\8_image_L86913-15.jpg</t>
-        </is>
-      </c>
-      <c r="C41" t="n">
-        <v>500</v>
-      </c>
-      <c r="D41" t="n">
-        <v>948</v>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>L86913-3</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L86913-3\7_image_L86913-3.jpg</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>500</v>
-      </c>
-      <c r="D42" t="n">
-        <v>948</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>L86963-10</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L86963-10\7_image_L86963-10.jpg</t>
-        </is>
-      </c>
-      <c r="C43" t="n">
-        <v>500</v>
-      </c>
-      <c r="D43" t="n">
-        <v>948</v>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>L86963-10</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L86963-10\8_image_L86963-10.jpg</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
-        <v>873</v>
-      </c>
-      <c r="D44" t="n">
-        <v>500</v>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>L86963-14</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\L86963-14\7_image_L86963-14.jpg</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
-        <v>500</v>
-      </c>
-      <c r="D45" t="n">
-        <v>948</v>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>LC45851X-2</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\LC45851X-2\1_image_LC45851X-2.jpg</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>724</v>
-      </c>
-      <c r="D46" t="n">
-        <v>500</v>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>LC47323-1</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\LC47323-1\1_image_LC47323-1.jpg</t>
-        </is>
-      </c>
-      <c r="C47" t="n">
-        <v>500</v>
-      </c>
-      <c r="D47" t="n">
-        <v>842</v>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>LC89049-F9976</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\LC89049-F9976\6_image_LC89049-F9976.jpg</t>
-        </is>
-      </c>
-      <c r="C48" t="n">
-        <v>1162</v>
-      </c>
-      <c r="D48" t="n">
-        <v>500</v>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>T37193-5056</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\T37193-5056\2_image_T37193-5056.jpg</t>
-        </is>
-      </c>
-      <c r="C49" t="n">
-        <v>500</v>
-      </c>
-      <c r="D49" t="n">
-        <v>1785</v>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>T37193-5056</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/21212\T37193-5056\4_image_T37193-5056.jpg</t>
-        </is>
-      </c>
-      <c r="C50" t="n">
-        <v>1169</v>
-      </c>
-      <c r="D50" t="n">
-        <v>500</v>
-      </c>
-      <c r="E50" t="inlineStr">
         <is>
           <t>min side 500 &lt; 501</t>
         </is>

</xml_diff>

<commit_message>
Auto update 2025-11-30 12:08:38
</commit_message>
<xml_diff>
--- a/bad_quality_photos.xlsx
+++ b/bad_quality_photos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,16 +451,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>L26835-51</t>
+          <t>100g1genw131-white</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\L26835-51\3_image_L26835-51.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\100g1genw131-white\001_image_100g1genw131-white.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>970</v>
+        <v>766</v>
       </c>
       <c r="D2" t="n">
         <v>500</v>
@@ -474,16 +474,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>L87530-4Y</t>
+          <t>100x1genw157-caramel</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\L87530-4Y\007_image_L87530-4Y.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\100x1genw157-caramel\1_image_100x1genw157-caramel.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>872</v>
+        <v>796</v>
       </c>
       <c r="D3" t="n">
         <v>500</v>
@@ -497,16 +497,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>L88005-215</t>
+          <t>110g1genw155-white</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\L88005-215\3_image_L88005-215.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\110g1genw155-white\1_image_110g1genw155-white.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>885</v>
+        <v>752</v>
       </c>
       <c r="D4" t="n">
         <v>500</v>
@@ -520,16 +520,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>L88530-1</t>
+          <t>110s1genw148-l</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\L88530-1\4_image_L88530-1.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\110s1genw148-lbrown\1_image_110s1genw148-l.brown.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>879</v>
+        <v>756</v>
       </c>
       <c r="D5" t="n">
         <v>500</v>
@@ -543,19 +543,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>L88542-1</t>
+          <t>110s1genw156-white</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\L88542-1\4_image_L88542-1.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\110s1genw156-white\2_image_110s1genw156-white.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>985</v>
+        <v>500</v>
       </c>
       <c r="D6" t="n">
-        <v>500</v>
+        <v>818</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -566,16 +566,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>L88542-65</t>
+          <t>11320400</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\L88542-65\007_image_L88542-65.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\11320400\001_image_11320400.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>833</v>
+        <v>978</v>
       </c>
       <c r="D7" t="n">
         <v>500</v>
@@ -589,16 +589,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LC14052-YP2020</t>
+          <t>115v1fx107-black</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC14052-YP2020\5_image_LC14052-YP2020.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\115v1fx107-black\001_image_115v1fx107-black.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>909</v>
+        <v>759</v>
       </c>
       <c r="D8" t="n">
         <v>500</v>
@@ -612,19 +612,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>LC14621-GD02</t>
+          <t>1173301</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC14621-GD02\009_image_LC14621-GD02.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\1173301\6_image_1173301.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>500</v>
+        <v>1299</v>
       </c>
       <c r="D9" t="n">
-        <v>847</v>
+        <v>500</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -635,16 +635,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LC14621-GD02</t>
+          <t>125v1fx107-black</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC14621-GD02\4_image_LC14621-GD02.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\125v1fx107-black\1_image_125v1fx107-black.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1029</v>
+        <v>759</v>
       </c>
       <c r="D10" t="n">
         <v>500</v>
@@ -658,19 +658,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LC14621-GD04</t>
+          <t>313512861</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC14621-GD04\7_image_LC14621-GD04.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\313512861\004_image_313512861.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>500</v>
+        <v>1528</v>
       </c>
       <c r="D11" t="n">
-        <v>1051</v>
+        <v>500</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -681,19 +681,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>LC14621-GD22</t>
+          <t>504161</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC14621-GD22\4_image_LC14621-GD22.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\504161\001_image_504161.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>828</v>
+        <v>500</v>
       </c>
       <c r="D12" t="n">
-        <v>500</v>
+        <v>538</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -704,16 +704,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>LC14621-GD25</t>
+          <t>5215801W</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC14621-GD25\5_image_LC14621-GD25.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\5215801W\011_image_5215801W.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1188</v>
+        <v>734</v>
       </c>
       <c r="D13" t="n">
         <v>500</v>
@@ -727,19 +727,19 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LC14621-GD25</t>
+          <t>5233401</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC14621-GD25\7_image_LC14621-GD25.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\5233401\4_image_5233401.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>500</v>
+        <v>569</v>
       </c>
       <c r="D14" t="n">
-        <v>911</v>
+        <v>500</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -750,16 +750,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>LC14805-GD01</t>
+          <t>5233401</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC14805-GD01\4_image_LC14805-GD01.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\5233401\7_image_5233401.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1062</v>
+        <v>777</v>
       </c>
       <c r="D15" t="n">
         <v>500</v>
@@ -773,16 +773,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>LC14825-GD01</t>
+          <t>5233401</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC14825-GD01\4_image_LC14825-GD01.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\5233401\8_image_5233401.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>955</v>
+        <v>748</v>
       </c>
       <c r="D16" t="n">
         <v>500</v>
@@ -796,16 +796,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LC68308-01</t>
+          <t>5236601</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC68308-01\4_image_LC68308-01.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\5236601\001_image_5236601.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>997</v>
+        <v>939</v>
       </c>
       <c r="D17" t="n">
         <v>500</v>
@@ -819,19 +819,19 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>LC68808-04</t>
+          <t>5243601</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC68808-04\008_image_LC68808-04.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\5243601\3_image_5243601.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>826</v>
+        <v>500</v>
       </c>
       <c r="D18" t="n">
-        <v>500</v>
+        <v>559</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -842,16 +842,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LC68900-05</t>
+          <t>545665</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC68900-05\001_image_LC68900-05.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\545665\2_image_545665.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>857</v>
+        <v>1068</v>
       </c>
       <c r="D19" t="n">
         <v>500</v>
@@ -865,16 +865,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LC68900-98</t>
+          <t>546661</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC68900-98\4_image_LC68900-98.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\546661\2_image_546661.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>992</v>
+        <v>1278</v>
       </c>
       <c r="D20" t="n">
         <v>500</v>
@@ -888,19 +888,19 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LC89049-F9976</t>
+          <t>739420</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\LC89049-F9976\6_image_LC89049-F9976.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\739420\001_image_739420.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1162</v>
+        <v>500</v>
       </c>
       <c r="D21" t="n">
-        <v>500</v>
+        <v>1137</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -911,19 +911,19 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>S31011-1</t>
+          <t>GA-0062-3md</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\S31011-1\001_image_S31011-1.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\GA-0062-3md\4_image_GA-0062-3md.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>719</v>
+        <v>500</v>
       </c>
       <c r="D22" t="n">
-        <v>500</v>
+        <v>1292</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -934,19 +934,19 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>S31578-2</t>
+          <t>GA-7290-3md</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\S31578-2\001_image_S31578-2.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\GA-7290-3md\003_image_GA-7290-3md.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>889</v>
+        <v>500</v>
       </c>
       <c r="D23" t="n">
-        <v>500</v>
+        <v>955</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -957,16 +957,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>S31585-7</t>
+          <t>GAlc-8033-4lx</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\S31585-7\001_image_S31585-7.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\GAlc-8033-4lx\6_image_GAlc-8033-4lx.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>909</v>
+        <v>998</v>
       </c>
       <c r="D24" t="n">
         <v>500</v>
@@ -980,19 +980,19 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>W15614-green</t>
+          <t>HB400A</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\W15614-green\001_image_W15614-green.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\HB400A\4_image_HB400A.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>858</v>
+        <v>500</v>
       </c>
       <c r="D25" t="n">
-        <v>500</v>
+        <v>1103</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1003,19 +1003,19 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Y-1088B-green</t>
+          <t>HB6154RB</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\Y-1088B-green\4_image_Y-1088B-green.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\HB6154RB\005_image_HB6154RB.jpg</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>905</v>
+        <v>500</v>
       </c>
       <c r="D26" t="n">
-        <v>500</v>
+        <v>554</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1026,19 +1026,19 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Y-7001A-lime-green-lak</t>
+          <t>Lim-181FA</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\Y-7001A-lime-green-lak\3_image_Y-7001A-lime-green-lak.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\Lim-181FA\6_image_Lim-181FA.jpg</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>924</v>
+        <v>500</v>
       </c>
       <c r="D27" t="n">
-        <v>500</v>
+        <v>1046</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1049,19 +1049,19 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Y-7001A-pink-lak</t>
+          <t>Lim-181RC</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\Y-7001A-pink-lak\3_image_Y-7001A-pink-lak.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\Lim-181RC\001_image_Lim-181RC.jpg</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>803</v>
+        <v>500</v>
       </c>
       <c r="D28" t="n">
-        <v>500</v>
+        <v>1095</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1072,19 +1072,19 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Y-7767A-deep-purple</t>
+          <t>Lim-181RC</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\Y-7767A-deep-purple\001_image_Y-7767A-deep-purple.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\Lim-181RC\3_image_Lim-181RC.jpg</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>940</v>
+        <v>500</v>
       </c>
       <c r="D29" t="n">
-        <v>500</v>
+        <v>1059</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1095,19 +1095,19 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Y-7767A-green</t>
+          <t>RB-2200L-4lx</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\Y-7767A-green\3_image_Y-7767A-green.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\RB-2200L-4lx\007_image_RB-2200L-4lx.jpg</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1006</v>
+        <v>500</v>
       </c>
       <c r="D30" t="n">
-        <v>500</v>
+        <v>1490</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1118,16 +1118,16 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Y-7767A-khaki</t>
+          <t>RB-3105-2lx</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\Y-7767A-khaki\001_image_Y-7767A-khaki.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\RB-3105-2lx\001_image_RB-3105-2lx.jpg</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>923</v>
+        <v>996</v>
       </c>
       <c r="D31" t="n">
         <v>500</v>
@@ -1141,21 +1141,113 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Y-7767A-red</t>
+          <t>RB-3105-3lx</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\Y-7767A-red\001_image_Y-7767A-red.jpg</t>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\RB-3105-3lx\001_image_RB-3105-3lx.jpg</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>938</v>
+        <v>996</v>
       </c>
       <c r="D32" t="n">
         <v>500</v>
       </c>
       <c r="E32" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>RC-6040-3md</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\RC-6040-3md\1_image_RC-6040-3md.jpg</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>500</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1065</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>RCg-1313-4lx</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\RCg-1313-4lx\5_image_RCg-1313-4lx.jpg</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1188</v>
+      </c>
+      <c r="D34" t="n">
+        <v>500</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>RE-8033-4lx</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\RE-8033-4lx\4_image_RE-8033-4lx.jpg</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>979</v>
+      </c>
+      <c r="D35" t="n">
+        <v>500</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>VC02816_Lblack</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/337/посортовані 337\VC02816_Lblack\002_image_VC02816_Lblack.jpg</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>500</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1141</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>min side 500 &lt; 501</t>
         </is>

</xml_diff>

<commit_message>
Auto update 2025-12-17 08:03:54
</commit_message>
<xml_diff>
--- a/bad_quality_photos.xlsx
+++ b/bad_quality_photos.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/не всі фото/обрізані фото\BN-GC-14-1-o-felt-d\2_image_BN-GC-14-1-o-felt-d-Photoroom.png</t>
+          <t>C:/Users/Asus/Desktop/не всі фото/обрізані фото\BN-GC-14-1-o-felt-d\2_image_BN-GC-14-1-o-felt-d-Photoroom.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -502,7 +502,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/не всі фото/обрізані фото\BN-SB-6\3_image_BN-SB-6_073926493725-Photoroom.png</t>
+          <t>C:/Users/Asus/Desktop/не всі фото/обрізані фото\BN-SB-6\3_image_BN-SB-6_073926493725-Photoroom.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">

</xml_diff>

<commit_message>
Auto update 2026-02-04 15:37:59
</commit_message>
<xml_diff>
--- a/bad_quality_photos.xlsx
+++ b/bad_quality_photos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,320 +451,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>522623</t>
+          <t>51411030m</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\522623\001_image_522623.jpg</t>
+          <t>C:/Users/Asus/Desktop/12\51411030m\3_image_51411030m.png</t>
         </is>
       </c>
       <c r="C2" t="n">
+        <v>909</v>
+      </c>
+      <c r="D2" t="n">
         <v>500</v>
       </c>
-      <c r="D2" t="n">
-        <v>700</v>
-      </c>
       <c r="E2" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>522660</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\522660\001_image_522660.jpg</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>500</v>
-      </c>
-      <c r="D3" t="n">
-        <v>710</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>BS70106-01</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\BS70106-01\5_image_BS70106-01.jpg</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>849</v>
-      </c>
-      <c r="D4" t="n">
-        <v>500</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>fz1896103</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\fz1896103\8_image_fz1896103.jpg</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>500</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1199</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>HB3628R</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\HB3628R\008_image_HB3628R.jpg</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>500</v>
-      </c>
-      <c r="D6" t="n">
-        <v>997</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>L28001-4</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\L28001-4\5_image_L28001-4.jpg</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1113</v>
-      </c>
-      <c r="D7" t="n">
-        <v>500</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>L28029-3</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\L28029-3\5_image_L28029-3.jpg</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>843</v>
-      </c>
-      <c r="D8" t="n">
-        <v>500</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>LC47991-1A</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\LC47991-1A\2_image_LC47991-1A.jpg</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1124</v>
-      </c>
-      <c r="D9" t="n">
-        <v>500</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>TW-CB-8-black</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\TW-CB-8-black\3_image_TW-CB-8-black.jpg</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>514</v>
-      </c>
-      <c r="D10" t="n">
-        <v>500</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>TW-OP-1-black</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\TW-OP-1-black\2_image_TW-OP-1-black.jpg</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>836</v>
-      </c>
-      <c r="D11" t="n">
-        <v>500</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>TW-OP-1-dark-blue</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\TW-OP-1-dark-blue\2_image_TW-OP-1-dark-blue.jpg</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>842</v>
-      </c>
-      <c r="D12" t="n">
-        <v>500</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>TW-OP-1-dark-blue</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\TW-OP-1-dark-blue\3_image_TW-OP-1-dark-blue.jpg</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>526</v>
-      </c>
-      <c r="D13" t="n">
-        <v>500</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>TW-OP-1-mars</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\TW-OP-1-mars\2_image_TW-OP-1-mars.jpg</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>830</v>
-      </c>
-      <c r="D14" t="n">
-        <v>500</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>min side 500 &lt; 501</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>TW-PM-Classic-mars</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/338/pfufkmyf gfgrf lkz akmk/посортовані для Гіт\TW-PM-Classic-mars\2_image_TW-PM-Classic-mars.jpg</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>500</v>
-      </c>
-      <c r="D15" t="n">
-        <v>749</v>
-      </c>
-      <c r="E15" t="inlineStr">
         <is>
           <t>min side 500 &lt; 501</t>
         </is>

</xml_diff>

<commit_message>
Auto update 2026-02-15 16:50:15
</commit_message>
<xml_diff>
--- a/bad_quality_photos.xlsx
+++ b/bad_quality_photos.xlsx
@@ -451,16 +451,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>51411030m</t>
+          <t>LC69055-76</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/12 — копия\51411030m\007_image_51411030m.jpg</t>
+          <t>C:/Users/Asus/Desktop/тест пнг\LC69055-76\5_image_LC69055-76.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>909</v>
+        <v>977</v>
       </c>
       <c r="D2" t="n">
         <v>500</v>
@@ -474,16 +474,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>51411030m</t>
+          <t>LC69802-01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/12 — копия\51411030m\007_image_51411030m.png</t>
+          <t>C:/Users/Asus/Desktop/тест пнг\LC69802-01\5_image_LC69802-01.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>909</v>
+        <v>1154</v>
       </c>
       <c r="D3" t="n">
         <v>500</v>

</xml_diff>

<commit_message>
Auto update 2026-02-18 09:50:35
</commit_message>
<xml_diff>
--- a/bad_quality_photos.xlsx
+++ b/bad_quality_photos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,16 +451,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LC69055-76</t>
+          <t>BN-BAG-17-choko-Photoroom</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/тест пнг\LC69055-76\5_image_LC69055-76.jpg</t>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\BN-BAG-17-choko\5_image_BN-BAG-17-choko-Photoroom.png</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>977</v>
+        <v>510</v>
       </c>
       <c r="D2" t="n">
         <v>500</v>
@@ -474,21 +474,297 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>BN-BAG-22-choko</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\BN-BAG-22-choko\005_image_BN-BAG-22-choko.jpg</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" t="n">
+        <v>604</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BN-BAG-28-choko</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\BN-BAG-28-choko\002_image_BN-BAG-28-choko.jpg</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>500</v>
+      </c>
+      <c r="D4" t="n">
+        <v>721</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BN-BAG-3-choko</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\BN-BAG-3-choko\002_image_BN-BAG-3-choko.jpg</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>500</v>
+      </c>
+      <c r="D5" t="n">
+        <v>602</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LC69055-76</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\LC69055-76\5_image_LC69055-76.jpg</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>977</v>
+      </c>
+      <c r="D6" t="n">
+        <v>500</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>LC69802-01</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>C:/Users/Asus/Desktop/тест пнг\LC69802-01\5_image_LC69802-01.jpg</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\LC69802-01\5_image_LC69802-01.jpg</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>1154</v>
       </c>
-      <c r="D3" t="n">
-        <v>500</v>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="D7" t="n">
+        <v>500</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LC69802-12</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\LC69802-12\009_image_LC69802-12.jpg</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>795</v>
+      </c>
+      <c r="D8" t="n">
+        <v>500</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>LC69802-12</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\LC69802-12\4_image_LC69802-12.jpg</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>866</v>
+      </c>
+      <c r="D9" t="n">
+        <v>500</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>LC69802-12</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\LC69802-12\5_image_LC69802-12.jpg</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1177</v>
+      </c>
+      <c r="D10" t="n">
+        <v>500</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LC69802-25</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\LC69802-25\001_image_LC69802-25.jpg</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>893</v>
+      </c>
+      <c r="D11" t="n">
+        <v>500</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>LC69802-25</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\LC69802-25\4_image_LC69802-25.jpg</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>897</v>
+      </c>
+      <c r="D12" t="n">
+        <v>500</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LC69855-2058</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\LC69855-2058\001_image_LC69855-2058.jpg</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>857</v>
+      </c>
+      <c r="D13" t="n">
+        <v>500</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>RCh-1313-4lx</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\RCh-1313-4lx\001_image_RCh-1313-4lx.jpg</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1183</v>
+      </c>
+      <c r="D14" t="n">
+        <v>500</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>min side 500 &lt; 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>TW-Lina-black-flo</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>C:/Users/Asus/Desktop/1 20.01.2026/339 фото/2 Новая папка обрізані\TW-Lina-black-flo\7_image_TW-Lina-black-flo.jpg</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>517</v>
+      </c>
+      <c r="D15" t="n">
+        <v>500</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>min side 500 &lt; 501</t>
         </is>

</xml_diff>